<commit_message>
Updated the status of the project in Gantt Chart
</commit_message>
<xml_diff>
--- a/GANTT CHART.xlsx
+++ b/GANTT CHART.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roshandev-my.sharepoint.com/personal/baingan_roshandev_onmicrosoft_com/Documents/codes/customer-retention/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{1A6923F2-D6B1-DA49-B2DA-D34DAABC4AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:20001_{1A6923F2-D6B1-DA49-B2DA-D34DAABC4AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A212EAC-26E8-D94E-BFCF-6B1B282F722B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -686,7 +685,7 @@
   <dimension ref="A1:AM1004"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -1583,7 +1582,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="22">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D14" s="23" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("IFERROR(SPARKLINE(C14,{""charttype"",""bar"";""color1"",""gray"";""max"",1}))"),"")</f>

</xml_diff>